<commit_message>
Add files for different work weeks
</commit_message>
<xml_diff>
--- a/gs170_ActionTracker-Marcos_Uc.xlsx
+++ b/gs170_ActionTracker-Marcos_Uc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muc\Desktop\uc\GS170\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299793A0-540C-46F4-BCA0-4310137CE020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E80C00-09BF-4E94-BAD6-636BA583E410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18015" yWindow="1845" windowWidth="11925" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Action Tracker" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="82">
   <si>
     <t xml:space="preserve">Applied for Job? </t>
   </si>
@@ -196,9 +196,6 @@
     <t>Area-Specific Strategies</t>
   </si>
   <si>
-    <t>Provide Details here on how you will accomplish this goal, what will you do each week to work toward accomplishing this goal?</t>
-  </si>
-  <si>
     <t>Weekly Contacts</t>
   </si>
   <si>
@@ -236,9 +233,6 @@
   </si>
   <si>
     <t xml:space="preserve">Met with professional to help understand the best area-specific strategies for me? </t>
-  </si>
-  <si>
-    <t>Write your specific goal here.</t>
   </si>
   <si>
     <t>Progress Toward Semester Goal</t>
@@ -283,6 +277,15 @@
   <si>
     <t>Other Skills/Resources Submitted for 
 Grading &amp; Feedback</t>
+  </si>
+  <si>
+    <t>My goal by the end of the semester will be to get my first web and computer programming certificate and apply for 5 job offers like a Front-End developer.</t>
+  </si>
+  <si>
+    <t>To achieve this goal, I will strengthen my networking and develop my presentation portfolio.                                                                                This is my me in 30 seconds: My name is Marcos Uc and I am a software engineer and a person passionate about technology, I skillfully develop myself in the Front-End area of all kinds of small or large pages, I really like learning about new technologies and I am constantly improving my skills in web development by taking online courses, I am a proactive person with high standards of work ethics, I like challenges and I am willing to give my best in the work area.</t>
+  </si>
+  <si>
+    <t>Currently I am aplying for job oportunities</t>
   </si>
 </sst>
 </file>
@@ -1122,8 +1125,8 @@
   </sheetPr>
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,14 +1146,14 @@
   <sheetData>
     <row r="1" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
       <c r="D1" s="53"/>
       <c r="E1" s="54"/>
       <c r="G1" s="52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H1" s="53"/>
       <c r="I1" s="53"/>
@@ -1160,7 +1163,7 @@
     </row>
     <row r="2" spans="1:12" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" s="49"/>
       <c r="C2" s="49"/>
@@ -1179,7 +1182,7 @@
     </row>
     <row r="3" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="56" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B3" s="57"/>
       <c r="C3" s="57"/>
@@ -1188,7 +1191,7 @@
         <v>21</v>
       </c>
       <c r="G3" s="58" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="H3" s="59"/>
       <c r="I3" s="59"/>
@@ -1215,7 +1218,7 @@
     </row>
     <row r="5" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="57"/>
       <c r="C5" s="57"/>
@@ -1234,7 +1237,7 @@
     </row>
     <row r="6" spans="1:12" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="56" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" s="57"/>
       <c r="C6" s="57"/>
@@ -1243,7 +1246,7 @@
         <v>21</v>
       </c>
       <c r="G6" s="58" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="H6" s="59"/>
       <c r="I6" s="59"/>
@@ -1270,14 +1273,14 @@
     </row>
     <row r="8" spans="1:12" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="47"/>
       <c r="C8" s="47"/>
       <c r="D8" s="47"/>
       <c r="E8" s="19">
         <f>(SUM('Action Tracker'!$C$23:$C$34))/20</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G8" s="58"/>
       <c r="H8" s="59"/>
@@ -1288,14 +1291,14 @@
     </row>
     <row r="9" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="47"/>
       <c r="C9" s="47"/>
       <c r="D9" s="47"/>
       <c r="E9" s="18">
         <f>SUM('Action Tracker'!$F$23:$F$34)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G9" s="58"/>
       <c r="H9" s="59"/>
@@ -1306,7 +1309,7 @@
     </row>
     <row r="10" spans="1:12" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B10" s="49"/>
       <c r="C10" s="49"/>
@@ -1323,7 +1326,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="46" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B11" s="47"/>
       <c r="C11" s="47"/>
@@ -1340,7 +1343,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="46" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B12" s="47"/>
       <c r="C12" s="47"/>
@@ -1357,7 +1360,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B13" s="47"/>
       <c r="C13" s="47"/>
@@ -1374,13 +1377,13 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="46" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B14" s="47"/>
       <c r="C14" s="47"/>
       <c r="D14" s="47"/>
       <c r="E14" s="20" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G14" s="58"/>
       <c r="H14" s="59"/>
@@ -1391,13 +1394,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="46" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B15" s="47"/>
       <c r="C15" s="47"/>
       <c r="D15" s="47"/>
       <c r="E15" s="20" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G15" s="58"/>
       <c r="H15" s="59"/>
@@ -1408,13 +1411,13 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B16" s="47"/>
       <c r="C16" s="47"/>
       <c r="D16" s="47"/>
       <c r="E16" s="20" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G16" s="58"/>
       <c r="H16" s="59"/>
@@ -1425,13 +1428,13 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="46" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B17" s="47"/>
       <c r="C17" s="47"/>
       <c r="D17" s="47"/>
       <c r="E17" s="20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G17" s="58"/>
       <c r="H17" s="59"/>
@@ -1442,13 +1445,13 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="50" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B18" s="51"/>
       <c r="C18" s="51"/>
       <c r="D18" s="51"/>
       <c r="E18" s="21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G18" s="61"/>
       <c r="H18" s="62"/>
@@ -1476,7 +1479,7 @@
     <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="66" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="66"/>
       <c r="D21" s="65"/>
@@ -1486,15 +1489,15 @@
       <c r="F21" s="66"/>
       <c r="G21" s="65"/>
       <c r="H21" s="64" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I21" s="65"/>
       <c r="J21" s="64" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="K21" s="65"/>
       <c r="L21" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1512,7 +1515,7 @@
         <v>15</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>13</v>
@@ -1556,14 +1559,20 @@
         <v>27</v>
       </c>
       <c r="H23" s="41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I23" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="J23" s="23"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
+      <c r="J23" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="K23" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="L23" s="24" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="24" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
@@ -1607,9 +1616,15 @@
       <c r="A26" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
+      <c r="B26" s="33">
+        <v>2</v>
+      </c>
+      <c r="C26" s="33">
+        <v>2</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>28</v>
+      </c>
       <c r="E26" s="34"/>
       <c r="F26" s="33"/>
       <c r="G26" s="33"/>
@@ -1623,12 +1638,24 @@
       <c r="A27" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="30"/>
+      <c r="B27" s="30">
+        <v>3</v>
+      </c>
+      <c r="C27" s="30">
+        <v>3</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="31">
+        <v>2</v>
+      </c>
+      <c r="F27" s="30">
+        <v>2</v>
+      </c>
+      <c r="G27" s="30" t="s">
+        <v>27</v>
+      </c>
       <c r="H27" s="32"/>
       <c r="I27" s="30"/>
       <c r="J27" s="32" t="s">
@@ -1637,7 +1664,9 @@
       <c r="K27" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="L27" s="28"/>
+      <c r="L27" s="28" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="28" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
@@ -1659,12 +1688,24 @@
       <c r="A29" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
+      <c r="B29" s="30">
+        <v>2</v>
+      </c>
+      <c r="C29" s="30">
+        <v>2</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="31">
+        <v>2</v>
+      </c>
+      <c r="F29" s="30">
+        <v>2</v>
+      </c>
+      <c r="G29" s="30" t="s">
+        <v>27</v>
+      </c>
       <c r="H29" s="32"/>
       <c r="I29" s="30"/>
       <c r="J29" s="32"/>
@@ -1675,9 +1716,15 @@
       <c r="A30" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
+      <c r="B30" s="33">
+        <v>2</v>
+      </c>
+      <c r="C30" s="33">
+        <v>2</v>
+      </c>
+      <c r="D30" s="33" t="s">
+        <v>27</v>
+      </c>
       <c r="E30" s="34"/>
       <c r="F30" s="33"/>
       <c r="G30" s="33"/>
@@ -1691,9 +1738,15 @@
       <c r="A31" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
+      <c r="B31" s="30">
+        <v>1</v>
+      </c>
+      <c r="C31" s="30">
+        <v>1</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>28</v>
+      </c>
       <c r="E31" s="31"/>
       <c r="F31" s="30"/>
       <c r="G31" s="30"/>
@@ -1939,7 +1992,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -1979,7 +2032,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
@@ -1996,10 +2049,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="C5" s="44" t="s">
         <v>11</v>

</xml_diff>